<commit_message>
getting weights into nice df
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="48">
   <si>
     <t>Index</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>EFA</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -223,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -247,12 +244,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -566,8 +557,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -611,315 +602,315 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>48</v>
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>48</v>
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>48</v>
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>48</v>
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>48</v>
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>48</v>
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>48</v>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>48</v>
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>48</v>
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>48</v>
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>48</v>
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>48</v>
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>48</v>
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>48</v>
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>48</v>
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>48</v>
+      <c r="A21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>48</v>
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>48</v>
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>48</v>
+      <c r="A24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>48</v>
+      <c r="A25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>48</v>
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>48</v>
+      <c r="A27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>48</v>
+      <c r="A28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>48</v>
+      <c r="A29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>48</v>
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>48</v>
+      <c r="A31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>48</v>
+      <c r="A32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>48</v>
+      <c r="A33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>48</v>
+      <c r="A34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>48</v>
+      <c r="A35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>48</v>
+      <c r="A36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>48</v>
+      <c r="A37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>48</v>
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>48</v>
+      <c r="A39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>48</v>
+      <c r="A40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>48</v>
+      <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>48</v>
+      <c r="A42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>48</v>
+      <c r="A43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>48</v>
+      <c r="A44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjustments to data and holdings
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="48">
   <si>
     <t>Index</t>
   </si>
@@ -551,7 +551,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -819,15 +819,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>33</v>
@@ -835,7 +835,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>33</v>
@@ -843,15 +843,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
@@ -859,7 +859,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>36</v>
@@ -867,7 +867,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>36</v>
@@ -875,7 +875,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>36</v>
@@ -883,7 +883,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>36</v>
@@ -891,7 +891,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>36</v>
@@ -899,17 +899,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusting constraints and logging
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="48">
   <si>
     <t>Index</t>
   </si>
@@ -551,7 +551,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -603,305 +603,105 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding a few more assets need to debug  returns
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="48">
   <si>
     <t>Index</t>
   </si>
@@ -551,7 +551,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -659,49 +659,113 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some more test cases
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="49">
   <si>
     <t>Index</t>
   </si>
@@ -158,7 +158,10 @@
     <t>SPY</t>
   </si>
   <si>
-    <t>EFA</t>
+    <t>TLT</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -244,6 +247,12 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -557,8 +566,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -582,191 +591,191 @@
         <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
+      <c r="A5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
+      <c r="A6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>20</v>
+      <c r="A8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
+      <c r="A9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
+      <c r="A10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
+      <c r="A11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
+      <c r="A12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
+      <c r="A13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
+      <c r="A14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>22</v>
+      <c r="A15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>33</v>
+      <c r="A16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
+      <c r="A17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>33</v>
+      <c r="A18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
+      <c r="A19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>36</v>
+      <c r="A20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>36</v>
+      <c r="A21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>36</v>
+      <c r="A22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>36</v>
+      <c r="A23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>36</v>
+      <c r="A24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>36</v>
+      <c r="A25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>36</v>
+      <c r="A26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making some changes to the sharpe ratio
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
   <si>
     <t>Index</t>
   </si>
@@ -548,7 +548,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -630,19 +630,11 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
-        <v>38</v>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more holdings see how we go!
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="45">
   <si>
     <t>Index</t>
   </si>
@@ -149,13 +149,7 @@
     <t>ACWI</t>
   </si>
   <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>SPY</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -217,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -240,7 +234,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -548,27 +545,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>45</v>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -576,66 +573,346 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="A32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="A35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+      <c r="A36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="A37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="A38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+      <c r="A39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="A40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+      <c r="A45" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to holdings file
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="75">
   <si>
     <t>Index</t>
   </si>
@@ -153,6 +153,93 @@
   </si>
   <si>
     <t>Industry</t>
+  </si>
+  <si>
+    <t>iShares iBoxx $ Inv Grade Corporate Bond ETF</t>
+  </si>
+  <si>
+    <t>iShares iBoxx $ High Yield Corporate Bond ETF</t>
+  </si>
+  <si>
+    <t>Vanguard Total Bond Market Index Fund ETF</t>
+  </si>
+  <si>
+    <t>iShares US Treasury Bond ETF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iShares Short Treasury Bond ETF</t>
+  </si>
+  <si>
+    <t>iShares TIPS Bond ETF</t>
+  </si>
+  <si>
+    <t>iShares US Aerospace &amp; Defense ETF</t>
+  </si>
+  <si>
+    <t>defense</t>
+  </si>
+  <si>
+    <t>iShares National Muni Bond ETF</t>
+  </si>
+  <si>
+    <t>SPDR Gold Trust</t>
+  </si>
+  <si>
+    <t>United States Oil ETF</t>
+  </si>
+  <si>
+    <t>Invesco DB Agriculture Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iShares Silver Trust</t>
+  </si>
+  <si>
+    <t>SPDR S&amp;P Metals &amp; Mining ETF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United States Natural Gas Fund, LP</t>
+  </si>
+  <si>
+    <t>Invesco DB Base Metals Fund</t>
+  </si>
+  <si>
+    <t>iShares S&amp;P GSCI Commodity-Indexed Trust ETF</t>
+  </si>
+  <si>
+    <t>United States Brent Oil Fund LP</t>
+  </si>
+  <si>
+    <t>SPDR S&amp;P Oil &amp; Gas Exploration &amp; Production ETF</t>
+  </si>
+  <si>
+    <t>SPDR Bloomberg 1-3 Month T-Bill ETF</t>
+  </si>
+  <si>
+    <t>iShares Treasury Floating Rate Bond ETF</t>
+  </si>
+  <si>
+    <t>Vanguard Total Stock Market Index Fund ETF</t>
+  </si>
+  <si>
+    <t>iShares Russell 2000 ETF</t>
+  </si>
+  <si>
+    <t>Nasdaq</t>
+  </si>
+  <si>
+    <t>iShares MSCI Emerging Markets ETF</t>
+  </si>
+  <si>
+    <t>SPDR Dow Jones Industrial Average ETF Trust</t>
+  </si>
+  <si>
+    <t>iShares Core S&amp;P Small-Cap ETF</t>
+  </si>
+  <si>
+    <t>iShares S&amp;P 500 Value ETF</t>
+  </si>
+  <si>
+    <t>iShares MSCI ACWI ETF mid cap from many countries</t>
   </si>
 </sst>
 </file>
@@ -160,7 +247,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +271,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -214,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -236,6 +329,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -545,29 +641,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="46.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -576,14 +677,20 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -592,14 +699,20 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -608,15 +721,21 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -624,288 +743,262 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>20</v>
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>57</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>20</v>
+      <c r="A18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>20</v>
+      <c r="A20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>22</v>
+      <c r="A22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>67</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>22</v>
+        <v>69</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>22</v>
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>22</v>
+        <v>71</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>22</v>
+      <c r="A28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>73</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>22</v>
+      <c r="A30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="A32" s="9"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="9"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>